<commit_message>
Final changes before chnaging frontend
</commit_message>
<xml_diff>
--- a/brand_data_hackathon.xlsx
+++ b/brand_data_hackathon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Regina\OneDrive\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F5352E-86FD-429B-965A-5409E451DC5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7EEC88-8AAE-4E0B-9BAA-969DE0D43A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{16862EFB-2D41-489E-A416-4615753F3809}"/>
   </bookViews>
@@ -515,10 +515,13 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -587,7 +590,7 @@
         <v>10700</v>
       </c>
       <c r="D5">
-        <v>2159.84</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -629,7 +632,7 @@
         <v>45000</v>
       </c>
       <c r="D8">
-        <v>7.69</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -657,7 +660,7 @@
         <v>30000</v>
       </c>
       <c r="D10">
-        <v>7.69</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -713,7 +716,7 @@
         <v>45000</v>
       </c>
       <c r="D14">
-        <v>7.69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -741,7 +744,7 @@
         <v>50000</v>
       </c>
       <c r="D16">
-        <v>7.69</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -783,7 +786,7 @@
         <v>24000</v>
       </c>
       <c r="D19">
-        <v>7.69</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -839,7 +842,7 @@
         <v>35000</v>
       </c>
       <c r="D23">
-        <v>7.69</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -881,7 +884,7 @@
         <v>22920</v>
       </c>
       <c r="D26">
-        <v>7.69</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -895,7 +898,7 @@
         <v>15000</v>
       </c>
       <c r="D27">
-        <v>7.69</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -937,7 +940,7 @@
         <v>50000</v>
       </c>
       <c r="D30">
-        <v>7.69</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -951,7 +954,7 @@
         <v>100000</v>
       </c>
       <c r="D31">
-        <v>7.69</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -965,7 +968,7 @@
         <v>100000</v>
       </c>
       <c r="D32">
-        <v>7.69</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>